<commit_message>
Gene Extractor Tiers 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/RedMattis/Gene Extractor Tiers - 3016454783/Gene Extractor Tiers - 3016454783.xlsx
+++ b/Data/RedMattis/Gene Extractor Tiers - 3016454783/Gene Extractor Tiers - 3016454783.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Gene Extractor Tiers - 3016454783\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E999F490-3C24-4ECB-AFD7-C2D5AD099C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC26955-8666-420D-9B1C-40A7437A9F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,681 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Lammergeier</author>
-  </authors>
-  <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E40" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E42" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E49" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E50" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 소실되었던 원문이 추가되었습니다.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-15에 새로 추가된 노드들 (9개)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000033000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2024-05-25에 새로 추가된 노드들 (22개)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="323">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1016,7 +343,7 @@
     <t>GET_GeneExtractor_IV.description</t>
   </si>
   <si>
-    <t>An automated surgery machine that can extract a person's genes and create a genepack from them, this version operates at 250% of the speed a regular extractor vat, but requires an AI persona core. The machine will slowly extract genes from the person in it, preferring genes not already stored nearby.\n\nA large amount of nutrition will be consumed while in use.\n\nThis version can extract archite genes.\n\nThese more advanced machines are capable of extracting genes from Baseliners, such as "Regular Sleeper" or "Human Hands"</t>
+    <t>Keyed+GET_TargetGene</t>
   </si>
   <si>
     <t>사람의 유전자를 추출하여 유전자 팩을 만들 수 있는 자동 수술 기계입니다. 이 기계는 일반 초월 유전자 추출 배양기보다 250% 빠른 속도로 작동하지만, 인공자아 핵이 필요합니다. 이 기계는 아직 저장되어 있지 않은 유전자를 우선적으로 추출하며, 배양기 내의 사람의 유전자를 천천히 추출합니다.\n\n사용하는 동안 많은 양의 영양분이 소비됩니다.\n\n이 버전은 초월입자 유전자를 추출할 수 있습니다.\n\n이 고급 기계는 일반인에게서 "보통 수면" 또는 "인간 손"과 같은 유전자를 추출할 수 있습니다.</t>
@@ -1242,9 +569,6 @@
   </si>
   <si>
     <t>regular-haired</t>
-  </si>
-  <si>
-    <t>GeneDef+GET_RegularHair.description</t>
   </si>
   <si>
     <r>
@@ -1259,22 +583,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>GeneDef+GET_RegularHair.description</t>
+  </si>
+  <si>
     <t>GET_RegularHair.description</t>
-  </si>
-  <si>
-    <t>GeneCategoryDef+Body_Size.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>Carriers of this gene have fairly regular hair.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1289,6 +601,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>GeneCategoryDef+Body_Size.label</t>
+  </si>
+  <si>
     <t>GeneCategoryDef</t>
   </si>
   <si>
@@ -1296,9 +611,6 @@
   </si>
   <si>
     <t>body size</t>
-  </si>
-  <si>
-    <t>Keyed+GET_DeactivateOverdrive</t>
   </si>
   <si>
     <r>
@@ -1313,13 +625,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+GET_DeactivateOverdrive</t>
+  </si>
+  <si>
     <t>GET_DeactivateOverdrive</t>
   </si>
   <si>
     <t>Deactivate Ovedrive</t>
-  </si>
-  <si>
-    <t>Keyed+GET_DeactivateOverdriveDesc</t>
   </si>
   <si>
     <r>
@@ -1334,6 +646,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+GET_DeactivateOverdriveDesc</t>
+  </si>
+  <si>
     <t>GET_DeactivateOverdriveDesc</t>
   </si>
   <si>
@@ -1350,9 +665,6 @@
   </si>
   <si>
     <t>Overdrive</t>
-  </si>
-  <si>
-    <t>Keyed+GET_ActivateOverdriveDesc</t>
   </si>
   <si>
     <r>
@@ -1367,6 +679,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+GET_ActivateOverdriveDesc</t>
+  </si>
+  <si>
     <t>GET_ActivateOverdriveDesc</t>
   </si>
   <si>
@@ -1383,9 +698,6 @@
   </si>
   <si>
     <t>Chance to seperate zero-cost genes to own pack</t>
-  </si>
-  <si>
-    <t>Keyed+GET_DidSplitZeroCost</t>
   </si>
   <si>
     <r>
@@ -1400,6 +712,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Keyed+GET_DidSplitZeroCost</t>
+  </si>
+  <si>
     <t>GET_DidSplitZeroCost</t>
   </si>
   <si>
@@ -1424,6 +739,18 @@
     <t>DesignatorDropdownGroupDef+GET_GeneNodeArchite.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GeneNodeArchite.label</t>
   </si>
   <si>
@@ -1433,6 +760,18 @@
     <t>ThingDef+GET_GN_Engineer.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 2</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Engineer.label</t>
   </si>
   <si>
@@ -1442,12 +781,27 @@
     <t>ThingDef+GET_GN_Engineer.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 -메카닉</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Engineer.description</t>
   </si>
   <si>
     <t>This black-market gene node grants access to basic engineering skill genes. To build it a number of gene packs will be traded as part of the building process.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드는 기본 엔지니어링 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_Druid.label</t>
   </si>
   <si>
@@ -1460,6 +814,18 @@
     <t>ThingDef+GET_GN_Druid.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 농부</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Druid.description</t>
   </si>
   <si>
@@ -1469,6 +835,18 @@
     <t>ThingDef+GET_GN_Intern.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>이 암시장 유전자 노드는 기본 농업 관련 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Intern.label</t>
   </si>
   <si>
@@ -1478,12 +856,27 @@
     <t>ThingDef+GET_GN_Intern.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 인턴</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Intern.description</t>
   </si>
   <si>
     <t>This black-market gene node grants access to basic science-oriented skill genes. To build it a number of gene packs will be traded as part of the building process.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드는 기초 과학 중심의 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_Culture.label</t>
   </si>
   <si>
@@ -1496,12 +889,27 @@
     <t>ThingDef+GET_GN_Culture.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 문화</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Culture.description</t>
   </si>
   <si>
     <t>This black-market gene node grants access to basic culture-oriented skill genes. To build it a number of gene packs will be traded as part of the building process.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드는 기본 문화 중심의 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_Warrior.label</t>
   </si>
   <si>
@@ -1514,12 +922,27 @@
     <t>ThingDef+GET_GN_Warrior.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 전사</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Warrior.description</t>
   </si>
   <si>
     <t>This black-market gene node grants access to basic combat-oriented skill genes. To build it a number of gene packs will be traded as part of the building process.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드에서는 기본 전투 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_BasicBody.label</t>
   </si>
   <si>
@@ -1532,6 +955,18 @@
     <t>ThingDef+GET_GN_BasicBody.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 신체</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_BasicBody.description</t>
   </si>
   <si>
@@ -1541,6 +976,18 @@
     <t>ThingDef+GET_GN_ViperSpecial.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>이 암시장 유전자 노드는 기본 신체 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 개의 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_ViperSpecial.label</t>
   </si>
   <si>
@@ -1550,12 +997,27 @@
     <t>ThingDef+GET_GN_ViperSpecial.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 바이퍼</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_ViperSpecial.description</t>
   </si>
   <si>
     <t>This black-market gene node grants access to partial gene data from VIPER's Lamia Xenotype. The dealer insists that it is a great deal. But alas, still no refunds.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드는 VIPER의 라미아 이종형에서 일부 유전자 데이터에 액세스할 수 있는 권한을 부여합니다. 딜러는 이것이 큰 거래라고 주장합니다. 하지만 아쉽게도 아직 환불은 되지 않습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_WeaknessOfMind.label</t>
   </si>
   <si>
@@ -1565,12 +1027,27 @@
     <t>ThingDef+GET_GN_WeaknessOfMind.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 작은 정신</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_WeaknessOfMind.description</t>
   </si>
   <si>
     <t>This black-market gene node contains a huge variety of genes intended to optimize metabolism at the cost of limiting mental capacities. No refunds.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드에는 정신 능력을 제한하는 대가로 신진대사를 최적화하기 위한 다양한 유전자가 포함되어 있습니다. 환불되지 않습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_WeaknessOfBody.label</t>
   </si>
   <si>
@@ -1583,12 +1060,27 @@
     <t>ThingDef+GET_GN_WeaknessOfBody.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 작은 신체</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_WeaknessOfBody.description</t>
   </si>
   <si>
     <t>This black-market gene node contains a huge variety of genes intended to optimize metabolism at the cost of limiting the capacity for some physical acts. No refunds.</t>
   </si>
   <si>
+    <t>이 암시장 유전자 노드에는 일부 신체 행위의 용량을 제한하는 대신 신진대사를 최적화하기 위한 다양한 유전자가 포함되어 있습니다. 환불되지 않습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+GET_GN_Experimental.label</t>
   </si>
   <si>
@@ -1601,98 +1093,85 @@
     <t>ThingDef+GET_GN_Experimental.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유전자 노드 - 실험</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GET_GN_Experimental.description</t>
   </si>
   <si>
     <t>"You can't do proper science without breaking a few eggs". No refunds.</t>
   </si>
   <si>
-    <t>유전자 노드</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 -메카닉</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 - 농부</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드는 기본 엔지니어링 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드는 기본 농업 관련 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 - 인턴</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드는 기초 과학 중심의 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
-  </si>
-  <si>
-    <t>유전자 노드 - 문화</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드는 기본 문화 중심의 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
-  </si>
-  <si>
-    <t>유전자 노드 - 전사</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드에서는 기본 전투 기술 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
-  </si>
-  <si>
-    <t>유전자 노드 - 신체</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드는 기본 신체 유전자에 대한 접근 권한을 부여합니다. 이를 구축하기 위해 여러 개의 유전자 팩이 구축 과정의 일부로 거래됩니다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 - 바이퍼</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드는 VIPER의 라미아 이종형에서 일부 유전자 데이터에 액세스할 수 있는 권한을 부여합니다. 딜러는 이것이 큰 거래라고 주장합니다. 하지만 아쉽게도 아직 환불은 되지 않습니다.</t>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드에는 정신 능력을 제한하는 대가로 신진대사를 최적화하기 위한 다양한 유전자가 포함되어 있습니다. 환불되지 않습니다.</t>
+    <t>“달걀 몇 개 깨보지 않고는 제대로 된 과학을 할 수 없다”는 말이 있습니다. 환불 불가.</t>
+  </si>
+  <si>
+    <t>An automated surgery machine that can extract a person's genes and create a genepack from them, this version permits targeting specific genes and also operates at 250% of the speed a regular extractor vat, but requires an AI persona core. The machine will slowly extract genes from the person in it, preferring genes not already stored nearby.\n\nA large amount of nutrition will be consumed while in use.\n\nThis version can extract archite genes.\n\nThese more advanced machines are capable of extracting genes from Baseliners, such as "Regular Sleeper" or "Human Hands"</t>
+  </si>
+  <si>
+    <t>GET_TargetGene</t>
+  </si>
+  <si>
+    <t>Target Gene: {0}</t>
+  </si>
+  <si>
+    <t>Keyed+GET_SelectGene</t>
+  </si>
+  <si>
+    <t>GET_SelectGene</t>
+  </si>
+  <si>
+    <t>Select Gene</t>
+  </si>
+  <si>
+    <t>Keyed+GET_SelectGeneDesc</t>
+  </si>
+  <si>
+    <t>GET_SelectGeneDesc</t>
+  </si>
+  <si>
+    <t>Select a specific gene for extraction.</t>
+  </si>
+  <si>
+    <t>Keyed+GET_AllVatsCanTargetGenes</t>
+  </si>
+  <si>
+    <t>GET_AllVatsCanTargetGenes</t>
+  </si>
+  <si>
+    <t>All Vats can Target specific genes.</t>
+  </si>
+  <si>
+    <t>대상 유전자: {0}</t>
+  </si>
+  <si>
+    <t>유전자 선택</t>
+  </si>
+  <si>
+    <t>추출할 특정 유전자를 선택하십시오.</t>
+  </si>
+  <si>
+    <t>모든 배양기는 특정 유전자를 대상으로 할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>Carriers of this gene have fairly regular hair.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Gene Node - Less Mind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 - 작은 정신</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 - 작은 신체</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 암시장 유전자 노드에는 일부 신체 행위의 용량을 제한하는 대신 신진대사를 최적화하기 위한 다양한 유전자가 포함되어 있습니다. 환불되지 않습니다.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Gene Node - Experimental</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 노드 - 실험</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>“달걀 몇 개 깨보지 않고는 제대로 된 과학을 할 수 없다”는 말이 있습니다. 환불 불가.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1713,34 +1192,26 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF87CEEB"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1755,11 +1226,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2061,11 +1531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2073,9 +1543,10 @@
     <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2091,7 +1562,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2517,7 +1988,7 @@
         <v>106</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>304</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>108</v>
@@ -2941,16 +2412,16 @@
       <c r="C52" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>182</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
@@ -2958,28 +2429,28 @@
       <c r="C53" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>187</v>
+      <c r="E53" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="E54" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2990,13 +2461,13 @@
         <v>156</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -3007,30 +2478,30 @@
         <v>156</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3041,30 +2512,30 @@
         <v>156</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -3075,47 +2546,47 @@
         <v>156</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="E61" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="F61" s="1" t="s">
-        <v>283</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="2" t="s">
         <v>223</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -3126,348 +2597,415 @@
         <v>85</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E63" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="E63" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="F63" s="1" t="s">
-        <v>285</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>287</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>288</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>247</v>
+        <v>254</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>253</v>
+        <v>262</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>294</v>
+        <v>264</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>256</v>
+        <v>266</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>259</v>
+        <v>270</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>262</v>
+        <v>274</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>265</v>
+        <v>278</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>300</v>
+        <v>282</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>270</v>
+        <v>285</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>273</v>
+        <v>289</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>276</v>
+        <v>293</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>282</v>
+        <v>298</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>306</v>
       </c>
+      <c r="F83" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>